<commit_message>
Arrows cap at 10; souls do not persist between rounds (updated tutorial), ante increases faster over time, river changes color as ante increases, hades patron buff, trials cannot appear twice in a run, obol of thorns nerfed
</commit_message>
<xml_diff>
--- a/assets/ante.xlsx
+++ b/assets/ante.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\Godot\Charon-s-Obol\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5477170B-AD13-4D80-B130-7CE8D884D266}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{909D4FA5-E764-4879-8971-5885F8D347B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{862E7D72-4771-4B74-8DB7-713B94245E6F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Triangular</t>
   </si>
@@ -60,6 +60,24 @@
   </si>
   <si>
     <t>Toss</t>
+  </si>
+  <si>
+    <t>Five</t>
+  </si>
+  <si>
+    <t>Five Sum</t>
+  </si>
+  <si>
+    <t>Six</t>
+  </si>
+  <si>
+    <t>Six Sum</t>
+  </si>
+  <si>
+    <t>Seven</t>
+  </si>
+  <si>
+    <t>Seven Sum</t>
   </si>
 </sst>
 </file>
@@ -431,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07F2D224-0D2C-43ED-A9A3-264035D20433}">
-  <dimension ref="A1:N8"/>
+  <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N26" sqref="N26"/>
+      <selection activeCell="S30" sqref="S30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -535,55 +553,55 @@
         <v>0</v>
       </c>
       <c r="B3">
-        <f>B2*(B2+1)/2</f>
+        <f t="shared" ref="B3:N3" si="0">B2*(B2+1)/2</f>
         <v>0</v>
       </c>
       <c r="C3">
-        <f>C2*(C2+1)/2</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="D3">
-        <f>D2*(D2+1)/2</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="E3">
-        <f>E2*(E2+1)/2</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="F3">
-        <f>F2*(F2+1)/2</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="G3">
-        <f>G2*(G2+1)/2</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="H3">
-        <f>H2*(H2+1)/2</f>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="I3">
-        <f>I2*(I2+1)/2</f>
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="J3">
-        <f>J2*(J2+1)/2</f>
+        <f t="shared" si="0"/>
         <v>36</v>
       </c>
       <c r="K3">
-        <f>K2*(K2+1)/2</f>
+        <f t="shared" si="0"/>
         <v>45</v>
       </c>
       <c r="L3">
-        <f>L2*(L2+1)/2</f>
+        <f t="shared" si="0"/>
         <v>55</v>
       </c>
       <c r="M3">
-        <f>M2*(M2+1)/2</f>
+        <f t="shared" si="0"/>
         <v>66</v>
       </c>
       <c r="N3">
-        <f>N2*(N2+1)/2</f>
+        <f t="shared" si="0"/>
         <v>78</v>
       </c>
     </row>
@@ -604,43 +622,43 @@
         <v>4</v>
       </c>
       <c r="E4">
-        <f t="shared" ref="E4:L4" si="0">D4+E3</f>
+        <f t="shared" ref="E4:L4" si="1">D4+E3</f>
         <v>10</v>
       </c>
       <c r="F4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="G4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>35</v>
       </c>
       <c r="H4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>56</v>
       </c>
       <c r="I4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>84</v>
       </c>
       <c r="J4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>120</v>
       </c>
       <c r="K4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>165</v>
       </c>
       <c r="L4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>220</v>
       </c>
       <c r="M4">
-        <f t="shared" ref="M4" si="1">L4+M3</f>
+        <f t="shared" ref="M4" si="2">L4+M3</f>
         <v>286</v>
       </c>
       <c r="N4">
-        <f t="shared" ref="N4" si="2">M4+N3</f>
+        <f t="shared" ref="N4" si="3">M4+N3</f>
         <v>364</v>
       </c>
     </row>
@@ -653,51 +671,51 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <f t="shared" ref="C5:N5" si="3">C2*3</f>
+        <f t="shared" ref="C5:N5" si="4">C2*3</f>
         <v>3</v>
       </c>
       <c r="D5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="E5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9</v>
       </c>
       <c r="F5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
       <c r="G5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
       <c r="H5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
       <c r="I5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>21</v>
       </c>
       <c r="J5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>24</v>
       </c>
       <c r="K5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>27</v>
       </c>
       <c r="L5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>30</v>
       </c>
       <c r="M5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>33</v>
       </c>
       <c r="N5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>36</v>
       </c>
     </row>
@@ -718,43 +736,43 @@
         <v>9</v>
       </c>
       <c r="E6">
-        <f t="shared" ref="E6:L6" si="4">E5+D6</f>
+        <f t="shared" ref="E6:L6" si="5">E5+D6</f>
         <v>18</v>
       </c>
       <c r="F6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>30</v>
       </c>
       <c r="G6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>45</v>
       </c>
       <c r="H6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>63</v>
       </c>
       <c r="I6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>84</v>
       </c>
       <c r="J6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>108</v>
       </c>
       <c r="K6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>135</v>
       </c>
       <c r="L6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>165</v>
       </c>
       <c r="M6">
-        <f t="shared" ref="M6" si="5">M5+L6</f>
+        <f t="shared" ref="M6" si="6">M5+L6</f>
         <v>198</v>
       </c>
       <c r="N6">
-        <f t="shared" ref="N6" si="6">N5+M6</f>
+        <f t="shared" ref="N6" si="7">N5+M6</f>
         <v>234</v>
       </c>
     </row>
@@ -767,51 +785,51 @@
         <v>0</v>
       </c>
       <c r="C7">
-        <f t="shared" ref="C7:N7" si="7">C2*4</f>
+        <f t="shared" ref="C7:N9" si="8">C2*4</f>
         <v>4</v>
       </c>
       <c r="D7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>8</v>
       </c>
       <c r="E7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>12</v>
       </c>
       <c r="F7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>16</v>
       </c>
       <c r="G7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>20</v>
       </c>
       <c r="H7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>24</v>
       </c>
       <c r="I7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>28</v>
       </c>
       <c r="J7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>32</v>
       </c>
       <c r="K7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>36</v>
       </c>
       <c r="L7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>40</v>
       </c>
       <c r="M7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>44</v>
       </c>
       <c r="N7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>48</v>
       </c>
     </row>
@@ -828,54 +846,396 @@
         <v>4</v>
       </c>
       <c r="D8">
-        <f t="shared" ref="D8:N8" si="8">D7+C8</f>
+        <f t="shared" ref="D8:N8" si="9">D7+C8</f>
         <v>12</v>
       </c>
       <c r="E8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>24</v>
       </c>
       <c r="F8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>40</v>
       </c>
       <c r="G8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>60</v>
       </c>
       <c r="H8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>84</v>
       </c>
       <c r="I8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>112</v>
       </c>
       <c r="J8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>144</v>
       </c>
       <c r="K8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>180</v>
       </c>
       <c r="L8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>220</v>
       </c>
       <c r="M8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>264</v>
       </c>
       <c r="N8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>312</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <f>B2*5</f>
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <f>C2*5</f>
+        <v>5</v>
+      </c>
+      <c r="D9">
+        <f t="shared" ref="D9:N9" si="10">D2*5</f>
+        <v>10</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="10"/>
+        <v>15</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="10"/>
+        <v>20</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="10"/>
+        <v>25</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="10"/>
+        <v>30</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="10"/>
+        <v>35</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="10"/>
+        <v>40</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="10"/>
+        <v>45</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="10"/>
+        <v>50</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="10"/>
+        <v>55</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="10"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <f>B9</f>
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <f>B10+C9</f>
+        <v>5</v>
+      </c>
+      <c r="D10">
+        <f>C10+D9</f>
+        <v>15</v>
+      </c>
+      <c r="E10">
+        <f t="shared" ref="E10:N10" si="11">D10+E9</f>
+        <v>30</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="11"/>
+        <v>50</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="11"/>
+        <v>75</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="11"/>
+        <v>105</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="11"/>
+        <v>140</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="11"/>
+        <v>180</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="11"/>
+        <v>225</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="11"/>
+        <v>275</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="11"/>
+        <v>330</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="11"/>
+        <v>390</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <f>B2*6</f>
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <f>C2*6</f>
+        <v>6</v>
+      </c>
+      <c r="D11">
+        <f t="shared" ref="D11:N11" si="12">D2*6</f>
+        <v>12</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="12"/>
+        <v>18</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="12"/>
+        <v>24</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="12"/>
+        <v>30</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="12"/>
+        <v>36</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="12"/>
+        <v>42</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="12"/>
+        <v>48</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="12"/>
+        <v>54</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="12"/>
+        <v>60</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="12"/>
+        <v>66</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="12"/>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <f>B11</f>
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <f>B12+C11</f>
+        <v>6</v>
+      </c>
+      <c r="D12">
+        <f t="shared" ref="D12:N12" si="13">C12+D11</f>
+        <v>18</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="13"/>
+        <v>36</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="13"/>
+        <v>60</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="13"/>
+        <v>90</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="13"/>
+        <v>126</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="13"/>
+        <v>168</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="13"/>
+        <v>216</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="13"/>
+        <v>270</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="13"/>
+        <v>330</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="13"/>
+        <v>396</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="13"/>
+        <v>468</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <f>B2*7</f>
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <f>C2*7</f>
+        <v>7</v>
+      </c>
+      <c r="D13">
+        <f t="shared" ref="D13:N13" si="14">D2*7</f>
+        <v>14</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="14"/>
+        <v>21</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="14"/>
+        <v>28</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="14"/>
+        <v>35</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="14"/>
+        <v>42</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="14"/>
+        <v>49</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="14"/>
+        <v>56</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="14"/>
+        <v>63</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="14"/>
+        <v>70</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="14"/>
+        <v>77</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="14"/>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <f>B13</f>
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <f>B14+C13</f>
+        <v>7</v>
+      </c>
+      <c r="D14">
+        <f t="shared" ref="D14:N14" si="15">C14+D13</f>
+        <v>21</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="15"/>
+        <v>42</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="15"/>
+        <v>70</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="15"/>
+        <v>105</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="15"/>
+        <v>147</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="15"/>
+        <v>196</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="15"/>
+        <v>252</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="15"/>
+        <v>315</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="15"/>
+        <v>385</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="15"/>
+        <v>462</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="15"/>
+        <v>546</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="B5:L5 B7 C7:N7" formula="1"/>
+    <ignoredError sqref="B5:L5 B7 C7:N7 M11:N11 B11:L11 B9 M13:N13 B13:L13" formula="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>